<commit_message>
Added Athlete and Rides Data to the excel sheet
</commit_message>
<xml_diff>
--- a/PQR data.xlsx
+++ b/PQR data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snidersa\git\CSSE-333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hernanre\git\CSSE-333(new)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115AD388-7777-43F7-AEE8-7099027E0EB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B67AEC-C958-4C82-9629-D546DE413986}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3648" yWindow="1992" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5460" yWindow="7230" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Broomstick" sheetId="1" r:id="rId1"/>
     <sheet name="Team" sheetId="2" r:id="rId2"/>
+    <sheet name="Athlete" sheetId="3" r:id="rId3"/>
+    <sheet name="Rides" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Stratus</t>
   </si>
@@ -53,6 +55,36 @@
   </si>
   <si>
     <t>Gribble</t>
+  </si>
+  <si>
+    <t>Hermione Granger</t>
+  </si>
+  <si>
+    <t>Ron Weasley</t>
+  </si>
+  <si>
+    <t>Albus Dumbledore</t>
+  </si>
+  <si>
+    <t>Ginny Weasley</t>
+  </si>
+  <si>
+    <t>Rubeus Hagrid</t>
+  </si>
+  <si>
+    <t>Minevra McGonagall</t>
+  </si>
+  <si>
+    <t>Gryfindor</t>
+  </si>
+  <si>
+    <t>Hufflepuff</t>
+  </si>
+  <si>
+    <t>Ravenclaw</t>
+  </si>
+  <si>
+    <t>Slytherin</t>
   </si>
 </sst>
 </file>
@@ -373,16 +405,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -393,7 +423,7 @@
         <v>43839</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -404,7 +434,7 @@
         <v>35841</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -415,7 +445,7 @@
         <v>40603</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
   </sheetData>
@@ -427,13 +457,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC46D71F-87DF-4C9B-9CF4-63FA226AAE5D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -444,7 +474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -453,6 +483,211 @@
       </c>
       <c r="C2" t="s">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0838B8-F0F5-4C91-AA9F-6796F92E38AB}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>4</v>
+      </c>
+      <c r="D1">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C8CC09-3B40-45FA-BBA9-EF888D43E84F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>